<commit_message>
Show result imgs in README.md
</commit_message>
<xml_diff>
--- a/curvatures_and_angles.xlsx
+++ b/curvatures_and_angles.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1113" uniqueCount="372">
   <si>
     <t>images</t>
   </si>
@@ -623,6 +623,513 @@
   </si>
   <si>
     <t>42.1021294564</t>
+  </si>
+  <si>
+    <t>0.7350057942322802</t>
+  </si>
+  <si>
+    <t>1.6158153848030807</t>
+  </si>
+  <si>
+    <t>1.194745687827511</t>
+  </si>
+  <si>
+    <t>-61.862805884348866</t>
+  </si>
+  <si>
+    <t>0.22706138461793562</t>
+  </si>
+  <si>
+    <t>46.639803052246904</t>
+  </si>
+  <si>
+    <t>0.4449941706742293</t>
+  </si>
+  <si>
+    <t>-40.66477975103772</t>
+  </si>
+  <si>
+    <t>0.3081079374274027</t>
+  </si>
+  <si>
+    <t>2.3589841596828705</t>
+  </si>
+  <si>
+    <t>0.5291785576608239</t>
+  </si>
+  <si>
+    <t>33.09037534150504</t>
+  </si>
+  <si>
+    <t>0.24548879595966153</t>
+  </si>
+  <si>
+    <t>-69.19882139313192</t>
+  </si>
+  <si>
+    <t>0.5166006071579928</t>
+  </si>
+  <si>
+    <t>-50.04377979250214</t>
+  </si>
+  <si>
+    <t>0.32421385220853155</t>
+  </si>
+  <si>
+    <t>30.377111979444223</t>
+  </si>
+  <si>
+    <t>0.7319709840985895</t>
+  </si>
+  <si>
+    <t>-56.35993995868019</t>
+  </si>
+  <si>
+    <t>0.29273456314858187</t>
+  </si>
+  <si>
+    <t>0.009180768322479948</t>
+  </si>
+  <si>
+    <t>0.30727762431444805</t>
+  </si>
+  <si>
+    <t>-75.27533018967797</t>
+  </si>
+  <si>
+    <t>0.4824479440586958</t>
+  </si>
+  <si>
+    <t>-40.87159507161345</t>
+  </si>
+  <si>
+    <t>0.7833183958982894</t>
+  </si>
+  <si>
+    <t>41.28087371596611</t>
+  </si>
+  <si>
+    <t>0.31103487569298344</t>
+  </si>
+  <si>
+    <t>-1.3584787472982558</t>
+  </si>
+  <si>
+    <t>0.41416334381238024</t>
+  </si>
+  <si>
+    <t>72.87548539863728</t>
+  </si>
+  <si>
+    <t>0.4647185339539222</t>
+  </si>
+  <si>
+    <t>-42.95392142389867</t>
+  </si>
+  <si>
+    <t>0.7416890866715237</t>
+  </si>
+  <si>
+    <t>57.87052714650813</t>
+  </si>
+  <si>
+    <t>1.5229097722731813</t>
+  </si>
+  <si>
+    <t>0.6598175247142395</t>
+  </si>
+  <si>
+    <t>2.2095551352757563</t>
+  </si>
+  <si>
+    <t>-49.35393536147338</t>
+  </si>
+  <si>
+    <t>0.5096970688199878</t>
+  </si>
+  <si>
+    <t>-44.89303709147492</t>
+  </si>
+  <si>
+    <t>0.9873925539283138</t>
+  </si>
+  <si>
+    <t>40.14495215830797</t>
+  </si>
+  <si>
+    <t>0.24573977535979996</t>
+  </si>
+  <si>
+    <t>45.48162748151636</t>
+  </si>
+  <si>
+    <t>0.6027505409792294</t>
+  </si>
+  <si>
+    <t>0.8649725842353726</t>
+  </si>
+  <si>
+    <t>1.491914888885308</t>
+  </si>
+  <si>
+    <t>-77.65903314806683</t>
+  </si>
+  <si>
+    <t>0.3227627350751532</t>
+  </si>
+  <si>
+    <t>36.5203062049753</t>
+  </si>
+  <si>
+    <t>0.45578046630912855</t>
+  </si>
+  <si>
+    <t>0.46291138167861484</t>
+  </si>
+  <si>
+    <t>0.23163886429306468</t>
+  </si>
+  <si>
+    <t>55.99169248348473</t>
+  </si>
+  <si>
+    <t>0.6222222363094299</t>
+  </si>
+  <si>
+    <t>-60.75542602305028</t>
+  </si>
+  <si>
+    <t>0.4532584071338404</t>
+  </si>
+  <si>
+    <t>45.93554795509133</t>
+  </si>
+  <si>
+    <t>0.24767241385953637</t>
+  </si>
+  <si>
+    <t>2.284317101728856</t>
+  </si>
+  <si>
+    <t>0.8114635589903915</t>
+  </si>
+  <si>
+    <t>-90.32458877157882</t>
+  </si>
+  <si>
+    <t>0.19529815655696647</t>
+  </si>
+  <si>
+    <t>-51.77018676496476</t>
+  </si>
+  <si>
+    <t>0.26446041206361126</t>
+  </si>
+  <si>
+    <t>40.35647077689208</t>
+  </si>
+  <si>
+    <t>0.7616997222362376</t>
+  </si>
+  <si>
+    <t>-45.761904200763794</t>
+  </si>
+  <si>
+    <t>0.7264958918244027</t>
+  </si>
+  <si>
+    <t>-0.4946817691279386</t>
+  </si>
+  <si>
+    <t>0.4814496282871457</t>
+  </si>
+  <si>
+    <t>-46.77389393166485</t>
+  </si>
+  <si>
+    <t>0.8765513448257034</t>
+  </si>
+  <si>
+    <t>41.007048665487766</t>
+  </si>
+  <si>
+    <t>0.931106740668793</t>
+  </si>
+  <si>
+    <t>42.1538277969265</t>
+  </si>
+  <si>
+    <t>0.6274849042648921</t>
+  </si>
+  <si>
+    <t>0.42591288217673506</t>
+  </si>
+  <si>
+    <t>0.1761645587174408</t>
+  </si>
+  <si>
+    <t>-41.07501270714483</t>
+  </si>
+  <si>
+    <t>0.4563008183384449</t>
+  </si>
+  <si>
+    <t>37.582794608302784</t>
+  </si>
+  <si>
+    <t>0.475711615975363</t>
+  </si>
+  <si>
+    <t>41.86980514878058</t>
+  </si>
+  <si>
+    <t>1.6158153848030812</t>
+  </si>
+  <si>
+    <t>-62.28070352662064</t>
+  </si>
+  <si>
+    <t>46.57267337894406</t>
+  </si>
+  <si>
+    <t>-40.43179532213934</t>
+  </si>
+  <si>
+    <t>2.3635951111378266</t>
+  </si>
+  <si>
+    <t>33.08576439005008</t>
+  </si>
+  <si>
+    <t>-69.25936900186454</t>
+  </si>
+  <si>
+    <t>-50.21144441452181</t>
+  </si>
+  <si>
+    <t>30.375153911711585</t>
+  </si>
+  <si>
+    <t>-55.941368719223334</t>
+  </si>
+  <si>
+    <t>0.2931612927891339</t>
+  </si>
+  <si>
+    <t>-75.55931071414463</t>
+  </si>
+  <si>
+    <t>-41.155575596080105</t>
+  </si>
+  <si>
+    <t>40.99689319149945</t>
+  </si>
+  <si>
+    <t>-1.3632746459871021</t>
+  </si>
+  <si>
+    <t>72.88028129732614</t>
+  </si>
+  <si>
+    <t>-42.982605299916735</t>
+  </si>
+  <si>
+    <t>57.87532304519698</t>
+  </si>
+  <si>
+    <t>0.6604244013047069</t>
+  </si>
+  <si>
+    <t>-49.35454223806385</t>
+  </si>
+  <si>
+    <t>-44.80289851755587</t>
+  </si>
+  <si>
+    <t>40.266803003582936</t>
+  </si>
+  <si>
+    <t>45.577346785988375</t>
+  </si>
+  <si>
+    <t>0.8622836727385236</t>
+  </si>
+  <si>
+    <t>-77.84089980187693</t>
+  </si>
+  <si>
+    <t>36.52299511647215</t>
+  </si>
+  <si>
+    <t>0.45256958767059086</t>
+  </si>
+  <si>
+    <t>56.060469651915646</t>
+  </si>
+  <si>
+    <t>-60.5477349032503</t>
+  </si>
+  <si>
+    <t>45.94588974909936</t>
+  </si>
+  <si>
+    <t>-89.8192943449941</t>
+  </si>
+  <si>
+    <t>40.22118736967285</t>
+  </si>
+  <si>
+    <t>-45.518298434030356</t>
+  </si>
+  <si>
+    <t>-0.49494994525445285</t>
+  </si>
+  <si>
+    <t>-46.72557882367181</t>
+  </si>
+  <si>
+    <t>41.63480020475689</t>
+  </si>
+  <si>
+    <t>42.15409597305302</t>
+  </si>
+  <si>
+    <t>0.4259128821767287</t>
+  </si>
+  <si>
+    <t>37.727672641425414</t>
+  </si>
+  <si>
+    <t>42.10065069569613</t>
+  </si>
+  <si>
+    <t>0.012008977419019377</t>
+  </si>
+  <si>
+    <t>-75.27815839877451</t>
+  </si>
+  <si>
+    <t>-41.69576091814054</t>
+  </si>
+  <si>
+    <t>41.27804550686957</t>
+  </si>
+  <si>
+    <t>-0.4895639815243696</t>
+  </si>
+  <si>
+    <t>-46.77901171926842</t>
+  </si>
+  <si>
+    <t>41.373440158542145</t>
+  </si>
+  <si>
+    <t>41.700731093441064</t>
+  </si>
+  <si>
+    <t>-1.360873264315293</t>
+  </si>
+  <si>
+    <t>72.87787991565432</t>
+  </si>
+  <si>
+    <t>-43.03406707177243</t>
+  </si>
+  <si>
+    <t>57.87292166352517</t>
+  </si>
+  <si>
+    <t>0.46141313480487894</t>
+  </si>
+  <si>
+    <t>56.051626104781356</t>
+  </si>
+  <si>
+    <t>-60.360909233760744</t>
+  </si>
+  <si>
+    <t>45.82351039185079</t>
+  </si>
+  <si>
+    <t>1.615815273063074</t>
+  </si>
+  <si>
+    <t>-62.213756356731025</t>
+  </si>
+  <si>
+    <t>46.25218574862876</t>
+  </si>
+  <si>
+    <t>-40.66477963929772</t>
+  </si>
+  <si>
+    <t>0.8568700641109782</t>
+  </si>
+  <si>
+    <t>-77.65093062794243</t>
+  </si>
+  <si>
+    <t>36.50525814334826</t>
+  </si>
+  <si>
+    <t>0.6604244013047005</t>
+  </si>
+  <si>
+    <t>-49.31638577281081</t>
+  </si>
+  <si>
+    <t>-44.71160627767274</t>
+  </si>
+  <si>
+    <t>40.02384257191041</t>
+  </si>
+  <si>
+    <t>45.55711204377421</t>
+  </si>
+  <si>
+    <t>2.363884652000043</t>
+  </si>
+  <si>
+    <t>32.86159818924267</t>
+  </si>
+  <si>
+    <t>-68.25662748305015</t>
+  </si>
+  <si>
+    <t>-49.990969481717485</t>
+  </si>
+  <si>
+    <t>30.37221148712705</t>
+  </si>
+  <si>
+    <t>-56.1491833698847</t>
+  </si>
+  <si>
+    <t>2.0636541433480198</t>
+  </si>
+  <si>
+    <t>-89.59863138661326</t>
+  </si>
+  <si>
+    <t>-51.937885498989466</t>
+  </si>
+  <si>
+    <t>40.44185032805368</t>
+  </si>
+  <si>
+    <t>-45.54124124238296</t>
+  </si>
+  <si>
+    <t>0.4232592627284058</t>
+  </si>
+  <si>
+    <t>-41.03902971010337</t>
+  </si>
+  <si>
+    <t>38.95719589102894</t>
+  </si>
+  <si>
+    <t>42.220715536540375</t>
   </si>
 </sst>
 </file>
@@ -954,7 +1461,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C212"/>
+  <dimension ref="A1:C371"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3292,6 +3799,1755 @@
         <v>202</v>
       </c>
     </row>
+    <row r="213" spans="1:3">
+      <c r="A213" t="s">
+        <v>0</v>
+      </c>
+      <c r="B213" t="s">
+        <v>1</v>
+      </c>
+      <c r="C213" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3">
+      <c r="A214" t="s">
+        <v>39</v>
+      </c>
+      <c r="B214" t="s">
+        <v>203</v>
+      </c>
+      <c r="C214" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3">
+      <c r="A215" t="s">
+        <v>39</v>
+      </c>
+      <c r="B215" t="s">
+        <v>205</v>
+      </c>
+      <c r="C215" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3">
+      <c r="A216" t="s">
+        <v>39</v>
+      </c>
+      <c r="B216" t="s">
+        <v>207</v>
+      </c>
+      <c r="C216" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3">
+      <c r="A217" t="s">
+        <v>39</v>
+      </c>
+      <c r="B217" t="s">
+        <v>209</v>
+      </c>
+      <c r="C217" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3">
+      <c r="A218" t="s">
+        <v>0</v>
+      </c>
+      <c r="B218" t="s">
+        <v>1</v>
+      </c>
+      <c r="C218" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3">
+      <c r="A219" t="s">
+        <v>66</v>
+      </c>
+      <c r="B219" t="s">
+        <v>211</v>
+      </c>
+      <c r="C219" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3">
+      <c r="A220" t="s">
+        <v>66</v>
+      </c>
+      <c r="B220" t="s">
+        <v>213</v>
+      </c>
+      <c r="C220" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3">
+      <c r="A221" t="s">
+        <v>66</v>
+      </c>
+      <c r="B221" t="s">
+        <v>215</v>
+      </c>
+      <c r="C221" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3">
+      <c r="A222" t="s">
+        <v>66</v>
+      </c>
+      <c r="B222" t="s">
+        <v>217</v>
+      </c>
+      <c r="C222" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3">
+      <c r="A223" t="s">
+        <v>66</v>
+      </c>
+      <c r="B223" t="s">
+        <v>219</v>
+      </c>
+      <c r="C223" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3">
+      <c r="A224" t="s">
+        <v>66</v>
+      </c>
+      <c r="B224" t="s">
+        <v>221</v>
+      </c>
+      <c r="C224" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3">
+      <c r="A225" t="s">
+        <v>0</v>
+      </c>
+      <c r="B225" t="s">
+        <v>1</v>
+      </c>
+      <c r="C225" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3">
+      <c r="A226" t="s">
+        <v>3</v>
+      </c>
+      <c r="B226" t="s">
+        <v>223</v>
+      </c>
+      <c r="C226" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3">
+      <c r="A227" t="s">
+        <v>3</v>
+      </c>
+      <c r="B227" t="s">
+        <v>225</v>
+      </c>
+      <c r="C227" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3">
+      <c r="A228" t="s">
+        <v>3</v>
+      </c>
+      <c r="B228" t="s">
+        <v>227</v>
+      </c>
+      <c r="C228" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3">
+      <c r="A229" t="s">
+        <v>3</v>
+      </c>
+      <c r="B229" t="s">
+        <v>229</v>
+      </c>
+      <c r="C229" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3">
+      <c r="A230" t="s">
+        <v>0</v>
+      </c>
+      <c r="B230" t="s">
+        <v>1</v>
+      </c>
+      <c r="C230" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3">
+      <c r="A231" t="s">
+        <v>21</v>
+      </c>
+      <c r="B231" t="s">
+        <v>231</v>
+      </c>
+      <c r="C231" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3">
+      <c r="A232" t="s">
+        <v>21</v>
+      </c>
+      <c r="B232" t="s">
+        <v>233</v>
+      </c>
+      <c r="C232" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3">
+      <c r="A233" t="s">
+        <v>21</v>
+      </c>
+      <c r="B233" t="s">
+        <v>235</v>
+      </c>
+      <c r="C233" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3">
+      <c r="A234" t="s">
+        <v>21</v>
+      </c>
+      <c r="B234" t="s">
+        <v>237</v>
+      </c>
+      <c r="C234" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3">
+      <c r="A235" t="s">
+        <v>0</v>
+      </c>
+      <c r="B235" t="s">
+        <v>1</v>
+      </c>
+      <c r="C235" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3">
+      <c r="A236" t="s">
+        <v>55</v>
+      </c>
+      <c r="B236" t="s">
+        <v>239</v>
+      </c>
+      <c r="C236" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3">
+      <c r="A237" t="s">
+        <v>55</v>
+      </c>
+      <c r="B237" t="s">
+        <v>241</v>
+      </c>
+      <c r="C237" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3">
+      <c r="A238" t="s">
+        <v>55</v>
+      </c>
+      <c r="B238" t="s">
+        <v>243</v>
+      </c>
+      <c r="C238" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3">
+      <c r="A239" t="s">
+        <v>55</v>
+      </c>
+      <c r="B239" t="s">
+        <v>245</v>
+      </c>
+      <c r="C239" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3">
+      <c r="A240" t="s">
+        <v>55</v>
+      </c>
+      <c r="B240" t="s">
+        <v>247</v>
+      </c>
+      <c r="C240" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3">
+      <c r="A241" t="s">
+        <v>0</v>
+      </c>
+      <c r="B241" t="s">
+        <v>1</v>
+      </c>
+      <c r="C241" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3">
+      <c r="A242" t="s">
+        <v>48</v>
+      </c>
+      <c r="B242" t="s">
+        <v>249</v>
+      </c>
+      <c r="C242" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3">
+      <c r="A243" t="s">
+        <v>48</v>
+      </c>
+      <c r="B243" t="s">
+        <v>251</v>
+      </c>
+      <c r="C243" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3">
+      <c r="A244" t="s">
+        <v>48</v>
+      </c>
+      <c r="B244" t="s">
+        <v>253</v>
+      </c>
+      <c r="C244" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3">
+      <c r="A245" t="s">
+        <v>0</v>
+      </c>
+      <c r="B245" t="s">
+        <v>1</v>
+      </c>
+      <c r="C245" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3">
+      <c r="A246" t="s">
+        <v>30</v>
+      </c>
+      <c r="B246" t="s">
+        <v>255</v>
+      </c>
+      <c r="C246" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3">
+      <c r="A247" t="s">
+        <v>30</v>
+      </c>
+      <c r="B247" t="s">
+        <v>257</v>
+      </c>
+      <c r="C247" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3">
+      <c r="A248" t="s">
+        <v>30</v>
+      </c>
+      <c r="B248" t="s">
+        <v>259</v>
+      </c>
+      <c r="C248" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3">
+      <c r="A249" t="s">
+        <v>30</v>
+      </c>
+      <c r="B249" t="s">
+        <v>261</v>
+      </c>
+      <c r="C249" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3">
+      <c r="A250" t="s">
+        <v>0</v>
+      </c>
+      <c r="B250" t="s">
+        <v>1</v>
+      </c>
+      <c r="C250" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3">
+      <c r="A251" t="s">
+        <v>79</v>
+      </c>
+      <c r="B251" t="s">
+        <v>263</v>
+      </c>
+      <c r="C251" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3">
+      <c r="A252" t="s">
+        <v>79</v>
+      </c>
+      <c r="B252" t="s">
+        <v>265</v>
+      </c>
+      <c r="C252" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3">
+      <c r="A253" t="s">
+        <v>79</v>
+      </c>
+      <c r="B253" t="s">
+        <v>267</v>
+      </c>
+      <c r="C253" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3">
+      <c r="A254" t="s">
+        <v>79</v>
+      </c>
+      <c r="B254" t="s">
+        <v>269</v>
+      </c>
+      <c r="C254" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3">
+      <c r="A255" t="s">
+        <v>79</v>
+      </c>
+      <c r="B255" t="s">
+        <v>271</v>
+      </c>
+      <c r="C255" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3">
+      <c r="A256" t="s">
+        <v>0</v>
+      </c>
+      <c r="B256" t="s">
+        <v>1</v>
+      </c>
+      <c r="C256" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3">
+      <c r="A257" t="s">
+        <v>12</v>
+      </c>
+      <c r="B257" t="s">
+        <v>273</v>
+      </c>
+      <c r="C257" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3">
+      <c r="A258" t="s">
+        <v>12</v>
+      </c>
+      <c r="B258" t="s">
+        <v>275</v>
+      </c>
+      <c r="C258" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3">
+      <c r="A259" t="s">
+        <v>12</v>
+      </c>
+      <c r="B259" t="s">
+        <v>277</v>
+      </c>
+      <c r="C259" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3">
+      <c r="A260" t="s">
+        <v>12</v>
+      </c>
+      <c r="B260" t="s">
+        <v>279</v>
+      </c>
+      <c r="C260" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3">
+      <c r="A261" t="s">
+        <v>0</v>
+      </c>
+      <c r="B261" t="s">
+        <v>1</v>
+      </c>
+      <c r="C261" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3">
+      <c r="A262" t="s">
+        <v>90</v>
+      </c>
+      <c r="B262" t="s">
+        <v>281</v>
+      </c>
+      <c r="C262" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3">
+      <c r="A263" t="s">
+        <v>90</v>
+      </c>
+      <c r="B263" t="s">
+        <v>283</v>
+      </c>
+      <c r="C263" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3">
+      <c r="A264" t="s">
+        <v>90</v>
+      </c>
+      <c r="B264" t="s">
+        <v>285</v>
+      </c>
+      <c r="C264" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3">
+      <c r="A265" t="s">
+        <v>90</v>
+      </c>
+      <c r="B265" t="s">
+        <v>287</v>
+      </c>
+      <c r="C265" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3">
+      <c r="A266" t="s">
+        <v>0</v>
+      </c>
+      <c r="B266" t="s">
+        <v>1</v>
+      </c>
+      <c r="C266" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3">
+      <c r="A267" t="s">
+        <v>39</v>
+      </c>
+      <c r="B267" t="s">
+        <v>203</v>
+      </c>
+      <c r="C267" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3">
+      <c r="A268" t="s">
+        <v>39</v>
+      </c>
+      <c r="B268" t="s">
+        <v>205</v>
+      </c>
+      <c r="C268" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3">
+      <c r="A269" t="s">
+        <v>39</v>
+      </c>
+      <c r="B269" t="s">
+        <v>207</v>
+      </c>
+      <c r="C269" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3">
+      <c r="A270" t="s">
+        <v>39</v>
+      </c>
+      <c r="B270" t="s">
+        <v>209</v>
+      </c>
+      <c r="C270" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3">
+      <c r="A271" t="s">
+        <v>0</v>
+      </c>
+      <c r="B271" t="s">
+        <v>1</v>
+      </c>
+      <c r="C271" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3">
+      <c r="A272" t="s">
+        <v>66</v>
+      </c>
+      <c r="B272" t="s">
+        <v>211</v>
+      </c>
+      <c r="C272" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3">
+      <c r="A273" t="s">
+        <v>66</v>
+      </c>
+      <c r="B273" t="s">
+        <v>213</v>
+      </c>
+      <c r="C273" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3">
+      <c r="A274" t="s">
+        <v>66</v>
+      </c>
+      <c r="B274" t="s">
+        <v>215</v>
+      </c>
+      <c r="C274" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3">
+      <c r="A275" t="s">
+        <v>66</v>
+      </c>
+      <c r="B275" t="s">
+        <v>217</v>
+      </c>
+      <c r="C275" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3">
+      <c r="A276" t="s">
+        <v>66</v>
+      </c>
+      <c r="B276" t="s">
+        <v>219</v>
+      </c>
+      <c r="C276" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3">
+      <c r="A277" t="s">
+        <v>66</v>
+      </c>
+      <c r="B277" t="s">
+        <v>221</v>
+      </c>
+      <c r="C277" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3">
+      <c r="A278" t="s">
+        <v>0</v>
+      </c>
+      <c r="B278" t="s">
+        <v>1</v>
+      </c>
+      <c r="C278" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3">
+      <c r="A279" t="s">
+        <v>3</v>
+      </c>
+      <c r="B279" t="s">
+        <v>223</v>
+      </c>
+      <c r="C279" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3">
+      <c r="A280" t="s">
+        <v>3</v>
+      </c>
+      <c r="B280" t="s">
+        <v>225</v>
+      </c>
+      <c r="C280" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3">
+      <c r="A281" t="s">
+        <v>3</v>
+      </c>
+      <c r="B281" t="s">
+        <v>227</v>
+      </c>
+      <c r="C281" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3">
+      <c r="A282" t="s">
+        <v>3</v>
+      </c>
+      <c r="B282" t="s">
+        <v>229</v>
+      </c>
+      <c r="C282" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3">
+      <c r="A283" t="s">
+        <v>0</v>
+      </c>
+      <c r="B283" t="s">
+        <v>1</v>
+      </c>
+      <c r="C283" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3">
+      <c r="A284" t="s">
+        <v>21</v>
+      </c>
+      <c r="B284" t="s">
+        <v>231</v>
+      </c>
+      <c r="C284" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3">
+      <c r="A285" t="s">
+        <v>21</v>
+      </c>
+      <c r="B285" t="s">
+        <v>233</v>
+      </c>
+      <c r="C285" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3">
+      <c r="A286" t="s">
+        <v>21</v>
+      </c>
+      <c r="B286" t="s">
+        <v>235</v>
+      </c>
+      <c r="C286" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3">
+      <c r="A287" t="s">
+        <v>21</v>
+      </c>
+      <c r="B287" t="s">
+        <v>237</v>
+      </c>
+      <c r="C287" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3">
+      <c r="A288" t="s">
+        <v>0</v>
+      </c>
+      <c r="B288" t="s">
+        <v>1</v>
+      </c>
+      <c r="C288" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3">
+      <c r="A289" t="s">
+        <v>55</v>
+      </c>
+      <c r="B289" t="s">
+        <v>239</v>
+      </c>
+      <c r="C289" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3">
+      <c r="A290" t="s">
+        <v>55</v>
+      </c>
+      <c r="B290" t="s">
+        <v>241</v>
+      </c>
+      <c r="C290" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3">
+      <c r="A291" t="s">
+        <v>55</v>
+      </c>
+      <c r="B291" t="s">
+        <v>243</v>
+      </c>
+      <c r="C291" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3">
+      <c r="A292" t="s">
+        <v>55</v>
+      </c>
+      <c r="B292" t="s">
+        <v>245</v>
+      </c>
+      <c r="C292" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3">
+      <c r="A293" t="s">
+        <v>55</v>
+      </c>
+      <c r="B293" t="s">
+        <v>247</v>
+      </c>
+      <c r="C293" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3">
+      <c r="A294" t="s">
+        <v>0</v>
+      </c>
+      <c r="B294" t="s">
+        <v>1</v>
+      </c>
+      <c r="C294" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="295" spans="1:3">
+      <c r="A295" t="s">
+        <v>48</v>
+      </c>
+      <c r="B295" t="s">
+        <v>249</v>
+      </c>
+      <c r="C295" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3">
+      <c r="A296" t="s">
+        <v>48</v>
+      </c>
+      <c r="B296" t="s">
+        <v>251</v>
+      </c>
+      <c r="C296" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3">
+      <c r="A297" t="s">
+        <v>48</v>
+      </c>
+      <c r="B297" t="s">
+        <v>253</v>
+      </c>
+      <c r="C297" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3">
+      <c r="A298" t="s">
+        <v>0</v>
+      </c>
+      <c r="B298" t="s">
+        <v>1</v>
+      </c>
+      <c r="C298" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="299" spans="1:3">
+      <c r="A299" t="s">
+        <v>30</v>
+      </c>
+      <c r="B299" t="s">
+        <v>255</v>
+      </c>
+      <c r="C299" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="300" spans="1:3">
+      <c r="A300" t="s">
+        <v>30</v>
+      </c>
+      <c r="B300" t="s">
+        <v>257</v>
+      </c>
+      <c r="C300" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="301" spans="1:3">
+      <c r="A301" t="s">
+        <v>30</v>
+      </c>
+      <c r="B301" t="s">
+        <v>259</v>
+      </c>
+      <c r="C301" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="302" spans="1:3">
+      <c r="A302" t="s">
+        <v>30</v>
+      </c>
+      <c r="B302" t="s">
+        <v>261</v>
+      </c>
+      <c r="C302" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="303" spans="1:3">
+      <c r="A303" t="s">
+        <v>0</v>
+      </c>
+      <c r="B303" t="s">
+        <v>1</v>
+      </c>
+      <c r="C303" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="304" spans="1:3">
+      <c r="A304" t="s">
+        <v>79</v>
+      </c>
+      <c r="B304" t="s">
+        <v>263</v>
+      </c>
+      <c r="C304" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="305" spans="1:3">
+      <c r="A305" t="s">
+        <v>79</v>
+      </c>
+      <c r="B305" t="s">
+        <v>265</v>
+      </c>
+      <c r="C305" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="306" spans="1:3">
+      <c r="A306" t="s">
+        <v>79</v>
+      </c>
+      <c r="B306" t="s">
+        <v>267</v>
+      </c>
+      <c r="C306" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="307" spans="1:3">
+      <c r="A307" t="s">
+        <v>79</v>
+      </c>
+      <c r="B307" t="s">
+        <v>269</v>
+      </c>
+      <c r="C307" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="308" spans="1:3">
+      <c r="A308" t="s">
+        <v>79</v>
+      </c>
+      <c r="B308" t="s">
+        <v>271</v>
+      </c>
+      <c r="C308" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="309" spans="1:3">
+      <c r="A309" t="s">
+        <v>0</v>
+      </c>
+      <c r="B309" t="s">
+        <v>1</v>
+      </c>
+      <c r="C309" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="310" spans="1:3">
+      <c r="A310" t="s">
+        <v>12</v>
+      </c>
+      <c r="B310" t="s">
+        <v>273</v>
+      </c>
+      <c r="C310" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="311" spans="1:3">
+      <c r="A311" t="s">
+        <v>12</v>
+      </c>
+      <c r="B311" t="s">
+        <v>275</v>
+      </c>
+      <c r="C311" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="312" spans="1:3">
+      <c r="A312" t="s">
+        <v>12</v>
+      </c>
+      <c r="B312" t="s">
+        <v>277</v>
+      </c>
+      <c r="C312" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="313" spans="1:3">
+      <c r="A313" t="s">
+        <v>12</v>
+      </c>
+      <c r="B313" t="s">
+        <v>279</v>
+      </c>
+      <c r="C313" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="314" spans="1:3">
+      <c r="A314" t="s">
+        <v>0</v>
+      </c>
+      <c r="B314" t="s">
+        <v>1</v>
+      </c>
+      <c r="C314" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="315" spans="1:3">
+      <c r="A315" t="s">
+        <v>90</v>
+      </c>
+      <c r="B315" t="s">
+        <v>281</v>
+      </c>
+      <c r="C315" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="316" spans="1:3">
+      <c r="A316" t="s">
+        <v>90</v>
+      </c>
+      <c r="B316" t="s">
+        <v>283</v>
+      </c>
+      <c r="C316" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="317" spans="1:3">
+      <c r="A317" t="s">
+        <v>90</v>
+      </c>
+      <c r="B317" t="s">
+        <v>285</v>
+      </c>
+      <c r="C317" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="318" spans="1:3">
+      <c r="A318" t="s">
+        <v>90</v>
+      </c>
+      <c r="B318" t="s">
+        <v>287</v>
+      </c>
+      <c r="C318" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="319" spans="1:3">
+      <c r="A319" t="s">
+        <v>0</v>
+      </c>
+      <c r="B319" t="s">
+        <v>1</v>
+      </c>
+      <c r="C319" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="320" spans="1:3">
+      <c r="A320" t="s">
+        <v>3</v>
+      </c>
+      <c r="B320" t="s">
+        <v>223</v>
+      </c>
+      <c r="C320" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="321" spans="1:3">
+      <c r="A321" t="s">
+        <v>3</v>
+      </c>
+      <c r="B321" t="s">
+        <v>225</v>
+      </c>
+      <c r="C321" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="322" spans="1:3">
+      <c r="A322" t="s">
+        <v>3</v>
+      </c>
+      <c r="B322" t="s">
+        <v>227</v>
+      </c>
+      <c r="C322" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="323" spans="1:3">
+      <c r="A323" t="s">
+        <v>3</v>
+      </c>
+      <c r="B323" t="s">
+        <v>229</v>
+      </c>
+      <c r="C323" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="324" spans="1:3">
+      <c r="A324" t="s">
+        <v>0</v>
+      </c>
+      <c r="B324" t="s">
+        <v>1</v>
+      </c>
+      <c r="C324" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="325" spans="1:3">
+      <c r="A325" t="s">
+        <v>12</v>
+      </c>
+      <c r="B325" t="s">
+        <v>273</v>
+      </c>
+      <c r="C325" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="326" spans="1:3">
+      <c r="A326" t="s">
+        <v>12</v>
+      </c>
+      <c r="B326" t="s">
+        <v>275</v>
+      </c>
+      <c r="C326" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="327" spans="1:3">
+      <c r="A327" t="s">
+        <v>12</v>
+      </c>
+      <c r="B327" t="s">
+        <v>277</v>
+      </c>
+      <c r="C327" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="328" spans="1:3">
+      <c r="A328" t="s">
+        <v>12</v>
+      </c>
+      <c r="B328" t="s">
+        <v>279</v>
+      </c>
+      <c r="C328" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="329" spans="1:3">
+      <c r="A329" t="s">
+        <v>0</v>
+      </c>
+      <c r="B329" t="s">
+        <v>1</v>
+      </c>
+      <c r="C329" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="330" spans="1:3">
+      <c r="A330" t="s">
+        <v>21</v>
+      </c>
+      <c r="B330" t="s">
+        <v>231</v>
+      </c>
+      <c r="C330" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="331" spans="1:3">
+      <c r="A331" t="s">
+        <v>21</v>
+      </c>
+      <c r="B331" t="s">
+        <v>233</v>
+      </c>
+      <c r="C331" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="332" spans="1:3">
+      <c r="A332" t="s">
+        <v>21</v>
+      </c>
+      <c r="B332" t="s">
+        <v>235</v>
+      </c>
+      <c r="C332" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="333" spans="1:3">
+      <c r="A333" t="s">
+        <v>21</v>
+      </c>
+      <c r="B333" t="s">
+        <v>237</v>
+      </c>
+      <c r="C333" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="334" spans="1:3">
+      <c r="A334" t="s">
+        <v>0</v>
+      </c>
+      <c r="B334" t="s">
+        <v>1</v>
+      </c>
+      <c r="C334" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="335" spans="1:3">
+      <c r="A335" t="s">
+        <v>30</v>
+      </c>
+      <c r="B335" t="s">
+        <v>255</v>
+      </c>
+      <c r="C335" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="336" spans="1:3">
+      <c r="A336" t="s">
+        <v>30</v>
+      </c>
+      <c r="B336" t="s">
+        <v>257</v>
+      </c>
+      <c r="C336" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="337" spans="1:3">
+      <c r="A337" t="s">
+        <v>30</v>
+      </c>
+      <c r="B337" t="s">
+        <v>259</v>
+      </c>
+      <c r="C337" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="338" spans="1:3">
+      <c r="A338" t="s">
+        <v>30</v>
+      </c>
+      <c r="B338" t="s">
+        <v>261</v>
+      </c>
+      <c r="C338" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="339" spans="1:3">
+      <c r="A339" t="s">
+        <v>0</v>
+      </c>
+      <c r="B339" t="s">
+        <v>1</v>
+      </c>
+      <c r="C339" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="340" spans="1:3">
+      <c r="A340" t="s">
+        <v>39</v>
+      </c>
+      <c r="B340" t="s">
+        <v>203</v>
+      </c>
+      <c r="C340" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="341" spans="1:3">
+      <c r="A341" t="s">
+        <v>39</v>
+      </c>
+      <c r="B341" t="s">
+        <v>205</v>
+      </c>
+      <c r="C341" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="342" spans="1:3">
+      <c r="A342" t="s">
+        <v>39</v>
+      </c>
+      <c r="B342" t="s">
+        <v>207</v>
+      </c>
+      <c r="C342" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="343" spans="1:3">
+      <c r="A343" t="s">
+        <v>39</v>
+      </c>
+      <c r="B343" t="s">
+        <v>209</v>
+      </c>
+      <c r="C343" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="344" spans="1:3">
+      <c r="A344" t="s">
+        <v>0</v>
+      </c>
+      <c r="B344" t="s">
+        <v>1</v>
+      </c>
+      <c r="C344" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="345" spans="1:3">
+      <c r="A345" t="s">
+        <v>48</v>
+      </c>
+      <c r="B345" t="s">
+        <v>249</v>
+      </c>
+      <c r="C345" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="346" spans="1:3">
+      <c r="A346" t="s">
+        <v>48</v>
+      </c>
+      <c r="B346" t="s">
+        <v>251</v>
+      </c>
+      <c r="C346" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="347" spans="1:3">
+      <c r="A347" t="s">
+        <v>48</v>
+      </c>
+      <c r="B347" t="s">
+        <v>253</v>
+      </c>
+      <c r="C347" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="348" spans="1:3">
+      <c r="A348" t="s">
+        <v>0</v>
+      </c>
+      <c r="B348" t="s">
+        <v>1</v>
+      </c>
+      <c r="C348" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="349" spans="1:3">
+      <c r="A349" t="s">
+        <v>55</v>
+      </c>
+      <c r="B349" t="s">
+        <v>239</v>
+      </c>
+      <c r="C349" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="350" spans="1:3">
+      <c r="A350" t="s">
+        <v>55</v>
+      </c>
+      <c r="B350" t="s">
+        <v>241</v>
+      </c>
+      <c r="C350" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="351" spans="1:3">
+      <c r="A351" t="s">
+        <v>55</v>
+      </c>
+      <c r="B351" t="s">
+        <v>243</v>
+      </c>
+      <c r="C351" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="352" spans="1:3">
+      <c r="A352" t="s">
+        <v>55</v>
+      </c>
+      <c r="B352" t="s">
+        <v>245</v>
+      </c>
+      <c r="C352" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="353" spans="1:3">
+      <c r="A353" t="s">
+        <v>55</v>
+      </c>
+      <c r="B353" t="s">
+        <v>247</v>
+      </c>
+      <c r="C353" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="354" spans="1:3">
+      <c r="A354" t="s">
+        <v>0</v>
+      </c>
+      <c r="B354" t="s">
+        <v>1</v>
+      </c>
+      <c r="C354" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="355" spans="1:3">
+      <c r="A355" t="s">
+        <v>66</v>
+      </c>
+      <c r="B355" t="s">
+        <v>211</v>
+      </c>
+      <c r="C355" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="356" spans="1:3">
+      <c r="A356" t="s">
+        <v>66</v>
+      </c>
+      <c r="B356" t="s">
+        <v>213</v>
+      </c>
+      <c r="C356" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="357" spans="1:3">
+      <c r="A357" t="s">
+        <v>66</v>
+      </c>
+      <c r="B357" t="s">
+        <v>215</v>
+      </c>
+      <c r="C357" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="358" spans="1:3">
+      <c r="A358" t="s">
+        <v>66</v>
+      </c>
+      <c r="B358" t="s">
+        <v>217</v>
+      </c>
+      <c r="C358" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="359" spans="1:3">
+      <c r="A359" t="s">
+        <v>66</v>
+      </c>
+      <c r="B359" t="s">
+        <v>219</v>
+      </c>
+      <c r="C359" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="360" spans="1:3">
+      <c r="A360" t="s">
+        <v>66</v>
+      </c>
+      <c r="B360" t="s">
+        <v>221</v>
+      </c>
+      <c r="C360" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="361" spans="1:3">
+      <c r="A361" t="s">
+        <v>0</v>
+      </c>
+      <c r="B361" t="s">
+        <v>1</v>
+      </c>
+      <c r="C361" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="362" spans="1:3">
+      <c r="A362" t="s">
+        <v>79</v>
+      </c>
+      <c r="B362" t="s">
+        <v>263</v>
+      </c>
+      <c r="C362" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="363" spans="1:3">
+      <c r="A363" t="s">
+        <v>79</v>
+      </c>
+      <c r="B363" t="s">
+        <v>265</v>
+      </c>
+      <c r="C363" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="364" spans="1:3">
+      <c r="A364" t="s">
+        <v>79</v>
+      </c>
+      <c r="B364" t="s">
+        <v>267</v>
+      </c>
+      <c r="C364" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="365" spans="1:3">
+      <c r="A365" t="s">
+        <v>79</v>
+      </c>
+      <c r="B365" t="s">
+        <v>269</v>
+      </c>
+      <c r="C365" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="366" spans="1:3">
+      <c r="A366" t="s">
+        <v>79</v>
+      </c>
+      <c r="B366" t="s">
+        <v>271</v>
+      </c>
+      <c r="C366" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="367" spans="1:3">
+      <c r="A367" t="s">
+        <v>0</v>
+      </c>
+      <c r="B367" t="s">
+        <v>1</v>
+      </c>
+      <c r="C367" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="368" spans="1:3">
+      <c r="A368" t="s">
+        <v>90</v>
+      </c>
+      <c r="B368" t="s">
+        <v>281</v>
+      </c>
+      <c r="C368" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="369" spans="1:3">
+      <c r="A369" t="s">
+        <v>90</v>
+      </c>
+      <c r="B369" t="s">
+        <v>283</v>
+      </c>
+      <c r="C369" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="370" spans="1:3">
+      <c r="A370" t="s">
+        <v>90</v>
+      </c>
+      <c r="B370" t="s">
+        <v>285</v>
+      </c>
+      <c r="C370" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="371" spans="1:3">
+      <c r="A371" t="s">
+        <v>90</v>
+      </c>
+      <c r="B371" t="s">
+        <v>287</v>
+      </c>
+      <c r="C371" t="s">
+        <v>371</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>